<commit_message>
Added atom labels in five languages
Added atom labels in five languages
- Chinese
- German
- Spanish
- French
- Italian
</commit_message>
<xml_diff>
--- a/src/docs/AtomsData.xlsx
+++ b/src/docs/AtomsData.xlsx
@@ -5959,9 +5959,6 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_33324</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:33331</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/CHEBI_33342</t>
   </si>
   <si>
@@ -6013,12 +6010,6 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_32594</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:33336</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:33369</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/CHEBI_49828</t>
   </si>
   <si>
@@ -6046,15 +6037,9 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_49648</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:33379</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/CHEBI_33380</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:33381</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/CHEBI_33382</t>
   </si>
   <si>
@@ -6076,24 +6061,6 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_49666</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:33364</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:29287</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:25195</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:30440</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:25016</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:33301</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/CHEBI_33313</t>
   </si>
   <si>
@@ -6112,15 +6079,9 @@
     <t>http://purl.obolibrary.org/obo/CHEBI_33337</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:33385</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/CHEBI_33386</t>
   </si>
   <si>
-    <t>http://purl.obolibrary.org/obo/CHEBI:27214</t>
-  </si>
-  <si>
     <t>http://purl.obolibrary.org/obo/CHEBI_33387</t>
   </si>
   <si>
@@ -6197,6 +6158,45 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/OCE_0000050</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_33331</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_33336</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_33369</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_33379</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_33381</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_33364</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_29287</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_25195</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_30440</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_25016</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_33301</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_33385</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/CHEBI_27214</t>
   </si>
 </sst>
 </file>
@@ -6515,8 +6515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CB119"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="E123" sqref="E123"/>
+    <sheetView tabSelected="1" topLeftCell="A86" workbookViewId="0">
+      <selection activeCell="E101" sqref="E101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -15149,7 +15149,7 @@
         <v>804</v>
       </c>
       <c r="D40" t="s">
-        <v>1974</v>
+        <v>2041</v>
       </c>
       <c r="E40" t="s">
         <v>67</v>
@@ -15364,7 +15364,7 @@
         <v>823</v>
       </c>
       <c r="D41" t="s">
-        <v>1975</v>
+        <v>1974</v>
       </c>
       <c r="E41" t="s">
         <v>67</v>
@@ -15579,7 +15579,7 @@
         <v>841</v>
       </c>
       <c r="D42" t="s">
-        <v>1976</v>
+        <v>1975</v>
       </c>
       <c r="E42" t="s">
         <v>67</v>
@@ -15794,7 +15794,7 @@
         <v>857</v>
       </c>
       <c r="D43" t="s">
-        <v>1977</v>
+        <v>1976</v>
       </c>
       <c r="E43" t="s">
         <v>67</v>
@@ -16009,7 +16009,7 @@
         <v>874</v>
       </c>
       <c r="D44" t="s">
-        <v>1978</v>
+        <v>1977</v>
       </c>
       <c r="E44" t="s">
         <v>93</v>
@@ -16209,7 +16209,7 @@
         <v>893</v>
       </c>
       <c r="D45" t="s">
-        <v>1979</v>
+        <v>1978</v>
       </c>
       <c r="E45" t="s">
         <v>67</v>
@@ -16427,7 +16427,7 @@
         <v>909</v>
       </c>
       <c r="D46" t="s">
-        <v>1980</v>
+        <v>1979</v>
       </c>
       <c r="E46" t="s">
         <v>67</v>
@@ -16642,7 +16642,7 @@
         <v>924</v>
       </c>
       <c r="D47" t="s">
-        <v>1981</v>
+        <v>1980</v>
       </c>
       <c r="E47" t="s">
         <v>67</v>
@@ -16863,7 +16863,7 @@
         <v>942</v>
       </c>
       <c r="D48" t="s">
-        <v>1982</v>
+        <v>1981</v>
       </c>
       <c r="E48" t="s">
         <v>67</v>
@@ -17084,7 +17084,7 @@
         <v>960</v>
       </c>
       <c r="D49" t="s">
-        <v>1983</v>
+        <v>1982</v>
       </c>
       <c r="E49" t="s">
         <v>67</v>
@@ -17305,7 +17305,7 @@
         <v>974</v>
       </c>
       <c r="D50" t="s">
-        <v>1984</v>
+        <v>1983</v>
       </c>
       <c r="E50" t="s">
         <v>67</v>
@@ -17523,7 +17523,7 @@
         <v>992</v>
       </c>
       <c r="D51" t="s">
-        <v>1985</v>
+        <v>1984</v>
       </c>
       <c r="E51" t="s">
         <v>67</v>
@@ -17741,7 +17741,7 @@
         <v>1013</v>
       </c>
       <c r="D52" t="s">
-        <v>1986</v>
+        <v>1985</v>
       </c>
       <c r="E52" t="s">
         <v>67</v>
@@ -17962,7 +17962,7 @@
         <v>1031</v>
       </c>
       <c r="D53" t="s">
-        <v>1987</v>
+        <v>1986</v>
       </c>
       <c r="E53" t="s">
         <v>67</v>
@@ -18177,7 +18177,7 @@
         <v>1049</v>
       </c>
       <c r="D54" t="s">
-        <v>1988</v>
+        <v>1987</v>
       </c>
       <c r="E54" t="s">
         <v>67</v>
@@ -18398,7 +18398,7 @@
         <v>1071</v>
       </c>
       <c r="D55" t="s">
-        <v>1989</v>
+        <v>1988</v>
       </c>
       <c r="E55" t="s">
         <v>93</v>
@@ -18613,7 +18613,7 @@
         <v>1083</v>
       </c>
       <c r="D56" t="s">
-        <v>1990</v>
+        <v>1989</v>
       </c>
       <c r="E56" t="s">
         <v>67</v>
@@ -18834,7 +18834,7 @@
         <v>1102</v>
       </c>
       <c r="D57" t="s">
-        <v>1991</v>
+        <v>1990</v>
       </c>
       <c r="E57" t="s">
         <v>67</v>
@@ -19052,7 +19052,7 @@
         <v>1120</v>
       </c>
       <c r="D58" t="s">
-        <v>1992</v>
+        <v>2042</v>
       </c>
       <c r="E58" t="s">
         <v>67</v>
@@ -19267,7 +19267,7 @@
         <v>1142</v>
       </c>
       <c r="D59" t="s">
-        <v>1993</v>
+        <v>2043</v>
       </c>
       <c r="E59" t="s">
         <v>67</v>
@@ -19479,7 +19479,7 @@
         <v>1161</v>
       </c>
       <c r="D60" t="s">
-        <v>1994</v>
+        <v>1991</v>
       </c>
       <c r="E60" t="s">
         <v>93</v>
@@ -19691,7 +19691,7 @@
         <v>1179</v>
       </c>
       <c r="D61" t="s">
-        <v>1995</v>
+        <v>1992</v>
       </c>
       <c r="E61" t="s">
         <v>93</v>
@@ -19900,7 +19900,7 @@
         <v>1195</v>
       </c>
       <c r="D62" t="s">
-        <v>1996</v>
+        <v>1993</v>
       </c>
       <c r="E62" t="s">
         <v>93</v>
@@ -20094,7 +20094,7 @@
         <v>1213</v>
       </c>
       <c r="D63" t="s">
-        <v>1997</v>
+        <v>1994</v>
       </c>
       <c r="E63" t="s">
         <v>93</v>
@@ -20303,7 +20303,7 @@
         <v>1230</v>
       </c>
       <c r="D64" t="s">
-        <v>1998</v>
+        <v>1995</v>
       </c>
       <c r="E64" t="s">
         <v>93</v>
@@ -20515,7 +20515,7 @@
         <v>1246</v>
       </c>
       <c r="D65" t="s">
-        <v>1999</v>
+        <v>1996</v>
       </c>
       <c r="E65" t="s">
         <v>93</v>
@@ -20724,7 +20724,7 @@
         <v>1263</v>
       </c>
       <c r="D66" t="s">
-        <v>2000</v>
+        <v>1997</v>
       </c>
       <c r="E66" t="s">
         <v>93</v>
@@ -20933,7 +20933,7 @@
         <v>1279</v>
       </c>
       <c r="D67" t="s">
-        <v>2001</v>
+        <v>1998</v>
       </c>
       <c r="E67" t="s">
         <v>93</v>
@@ -21148,7 +21148,7 @@
         <v>1295</v>
       </c>
       <c r="D68" t="s">
-        <v>2002</v>
+        <v>1999</v>
       </c>
       <c r="E68" t="s">
         <v>93</v>
@@ -21357,7 +21357,7 @@
         <v>1311</v>
       </c>
       <c r="D69" t="s">
-        <v>2003</v>
+        <v>2044</v>
       </c>
       <c r="E69" t="s">
         <v>67</v>
@@ -21566,7 +21566,7 @@
         <v>1327</v>
       </c>
       <c r="D70" t="s">
-        <v>2004</v>
+        <v>2000</v>
       </c>
       <c r="E70" t="s">
         <v>93</v>
@@ -21781,7 +21781,7 @@
         <v>1342</v>
       </c>
       <c r="D71" t="s">
-        <v>2005</v>
+        <v>2045</v>
       </c>
       <c r="E71" t="s">
         <v>93</v>
@@ -21993,7 +21993,7 @@
         <v>1358</v>
       </c>
       <c r="D72" t="s">
-        <v>2006</v>
+        <v>2001</v>
       </c>
       <c r="E72" t="s">
         <v>93</v>
@@ -22199,7 +22199,7 @@
         <v>1375</v>
       </c>
       <c r="D73" t="s">
-        <v>2007</v>
+        <v>2002</v>
       </c>
       <c r="E73" t="s">
         <v>93</v>
@@ -22414,7 +22414,7 @@
         <v>1388</v>
       </c>
       <c r="D74" t="s">
-        <v>2008</v>
+        <v>2003</v>
       </c>
       <c r="E74" t="s">
         <v>67</v>
@@ -22626,7 +22626,7 @@
         <v>1405</v>
       </c>
       <c r="D75" t="s">
-        <v>2009</v>
+        <v>2004</v>
       </c>
       <c r="E75" t="s">
         <v>67</v>
@@ -22826,7 +22826,7 @@
         <v>1424</v>
       </c>
       <c r="D76" t="s">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="E76" t="s">
         <v>93</v>
@@ -23032,7 +23032,7 @@
         <v>1439</v>
       </c>
       <c r="D77" t="s">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="E77" t="s">
         <v>67</v>
@@ -23238,7 +23238,7 @@
         <v>1454</v>
       </c>
       <c r="D78" t="s">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="E78" t="s">
         <v>67</v>
@@ -23450,7 +23450,7 @@
         <v>1467</v>
       </c>
       <c r="D79" t="s">
-        <v>2013</v>
+        <v>2046</v>
       </c>
       <c r="E79" t="s">
         <v>67</v>
@@ -23665,7 +23665,7 @@
         <v>1480</v>
       </c>
       <c r="D80" t="s">
-        <v>2014</v>
+        <v>2047</v>
       </c>
       <c r="E80" t="s">
         <v>67</v>
@@ -23886,7 +23886,7 @@
         <v>1497</v>
       </c>
       <c r="D81" t="s">
-        <v>2015</v>
+        <v>2048</v>
       </c>
       <c r="E81" t="s">
         <v>67</v>
@@ -24104,7 +24104,7 @@
         <v>1513</v>
       </c>
       <c r="D82" t="s">
-        <v>2016</v>
+        <v>2049</v>
       </c>
       <c r="E82" t="s">
         <v>67</v>
@@ -24319,7 +24319,7 @@
         <v>1529</v>
       </c>
       <c r="D83" t="s">
-        <v>2017</v>
+        <v>2050</v>
       </c>
       <c r="E83" t="s">
         <v>67</v>
@@ -24537,7 +24537,7 @@
         <v>1546</v>
       </c>
       <c r="D84" t="s">
-        <v>2018</v>
+        <v>2051</v>
       </c>
       <c r="E84" t="s">
         <v>67</v>
@@ -24755,7 +24755,7 @@
         <v>1561</v>
       </c>
       <c r="D85" t="s">
-        <v>2019</v>
+        <v>2008</v>
       </c>
       <c r="E85" t="s">
         <v>93</v>
@@ -24952,7 +24952,7 @@
         <v>1578</v>
       </c>
       <c r="D86" t="s">
-        <v>2020</v>
+        <v>2009</v>
       </c>
       <c r="E86" t="s">
         <v>93</v>
@@ -25116,7 +25116,7 @@
         <v>1589</v>
       </c>
       <c r="D87" t="s">
-        <v>2021</v>
+        <v>2010</v>
       </c>
       <c r="E87" t="s">
         <v>93</v>
@@ -25298,7 +25298,7 @@
         <v>1600</v>
       </c>
       <c r="D88" t="s">
-        <v>2022</v>
+        <v>2011</v>
       </c>
       <c r="E88" t="s">
         <v>93</v>
@@ -25465,7 +25465,7 @@
         <v>1611</v>
       </c>
       <c r="D89" t="s">
-        <v>2023</v>
+        <v>2012</v>
       </c>
       <c r="E89" t="s">
         <v>93</v>
@@ -25647,7 +25647,7 @@
         <v>1624</v>
       </c>
       <c r="D90" t="s">
-        <v>2024</v>
+        <v>2013</v>
       </c>
       <c r="E90" t="s">
         <v>93</v>
@@ -25841,7 +25841,7 @@
         <v>1641</v>
       </c>
       <c r="D91" t="s">
-        <v>2025</v>
+        <v>2052</v>
       </c>
       <c r="E91" t="s">
         <v>67</v>
@@ -26047,7 +26047,7 @@
         <v>1655</v>
       </c>
       <c r="D92" t="s">
-        <v>2026</v>
+        <v>2014</v>
       </c>
       <c r="E92" t="s">
         <v>93</v>
@@ -26235,7 +26235,7 @@
         <v>1667</v>
       </c>
       <c r="D93" t="s">
-        <v>2027</v>
+        <v>2053</v>
       </c>
       <c r="E93" t="s">
         <v>67</v>
@@ -26444,7 +26444,7 @@
         <v>1685</v>
       </c>
       <c r="D94" t="s">
-        <v>2028</v>
+        <v>2015</v>
       </c>
       <c r="E94" t="s">
         <v>93</v>
@@ -26617,7 +26617,7 @@
         <v>1699</v>
       </c>
       <c r="D95" t="s">
-        <v>2029</v>
+        <v>2016</v>
       </c>
       <c r="E95" t="s">
         <v>93</v>
@@ -26796,7 +26796,7 @@
         <v>1712</v>
       </c>
       <c r="D96" t="s">
-        <v>2030</v>
+        <v>2017</v>
       </c>
       <c r="E96" t="s">
         <v>93</v>
@@ -26969,7 +26969,7 @@
         <v>1726</v>
       </c>
       <c r="D97" t="s">
-        <v>2031</v>
+        <v>2018</v>
       </c>
       <c r="E97" t="s">
         <v>93</v>
@@ -27142,7 +27142,7 @@
         <v>1738</v>
       </c>
       <c r="D98" t="s">
-        <v>2032</v>
+        <v>2019</v>
       </c>
       <c r="E98" t="s">
         <v>93</v>
@@ -27309,7 +27309,7 @@
         <v>1749</v>
       </c>
       <c r="D99" t="s">
-        <v>2033</v>
+        <v>2020</v>
       </c>
       <c r="E99" t="s">
         <v>93</v>
@@ -27473,7 +27473,7 @@
         <v>1759</v>
       </c>
       <c r="D100" t="s">
-        <v>2034</v>
+        <v>2021</v>
       </c>
       <c r="E100" t="s">
         <v>93</v>
@@ -27616,7 +27616,7 @@
         <v>1768</v>
       </c>
       <c r="D101" t="s">
-        <v>2035</v>
+        <v>2022</v>
       </c>
       <c r="E101" t="s">
         <v>93</v>
@@ -27753,7 +27753,7 @@
         <v>1776</v>
       </c>
       <c r="D102" t="s">
-        <v>2036</v>
+        <v>2023</v>
       </c>
       <c r="E102" t="s">
         <v>93</v>
@@ -27890,7 +27890,7 @@
         <v>1785</v>
       </c>
       <c r="D103" t="s">
-        <v>2037</v>
+        <v>2024</v>
       </c>
       <c r="E103" t="s">
         <v>93</v>
@@ -28030,7 +28030,7 @@
         <v>1794</v>
       </c>
       <c r="D104" t="s">
-        <v>2038</v>
+        <v>2025</v>
       </c>
       <c r="E104" t="s">
         <v>93</v>
@@ -28158,7 +28158,7 @@
         <v>1804</v>
       </c>
       <c r="D105" t="s">
-        <v>2039</v>
+        <v>2026</v>
       </c>
       <c r="E105" t="s">
         <v>93</v>
@@ -28277,7 +28277,7 @@
         <v>1813</v>
       </c>
       <c r="D106" t="s">
-        <v>2040</v>
+        <v>2027</v>
       </c>
       <c r="E106" t="s">
         <v>93</v>
@@ -28396,7 +28396,7 @@
         <v>1821</v>
       </c>
       <c r="D107" t="s">
-        <v>2041</v>
+        <v>2028</v>
       </c>
       <c r="E107" t="s">
         <v>93</v>
@@ -28515,7 +28515,7 @@
         <v>1830</v>
       </c>
       <c r="D108" t="s">
-        <v>2042</v>
+        <v>2029</v>
       </c>
       <c r="E108" t="s">
         <v>93</v>
@@ -28634,7 +28634,7 @@
         <v>1839</v>
       </c>
       <c r="D109" t="s">
-        <v>2043</v>
+        <v>2030</v>
       </c>
       <c r="E109" t="s">
         <v>93</v>
@@ -28753,7 +28753,7 @@
         <v>1848</v>
       </c>
       <c r="D110" t="s">
-        <v>2044</v>
+        <v>2031</v>
       </c>
       <c r="E110" t="s">
         <v>93</v>
@@ -28872,7 +28872,7 @@
         <v>1857</v>
       </c>
       <c r="D111" t="s">
-        <v>2045</v>
+        <v>2032</v>
       </c>
       <c r="E111" t="s">
         <v>93</v>
@@ -28991,7 +28991,7 @@
         <v>1865</v>
       </c>
       <c r="D112" t="s">
-        <v>2046</v>
+        <v>2033</v>
       </c>
       <c r="E112" t="s">
         <v>93</v>
@@ -29110,7 +29110,7 @@
         <v>1873</v>
       </c>
       <c r="D113" t="s">
-        <v>2047</v>
+        <v>2034</v>
       </c>
       <c r="E113" t="s">
         <v>93</v>
@@ -29229,7 +29229,7 @@
         <v>1882</v>
       </c>
       <c r="D114" t="s">
-        <v>2048</v>
+        <v>2035</v>
       </c>
       <c r="E114" t="s">
         <v>93</v>
@@ -29318,7 +29318,7 @@
         <v>1882</v>
       </c>
       <c r="D115" t="s">
-        <v>2049</v>
+        <v>2036</v>
       </c>
       <c r="E115" t="s">
         <v>93</v>
@@ -29437,7 +29437,7 @@
         <v>1882</v>
       </c>
       <c r="D116" t="s">
-        <v>2050</v>
+        <v>2037</v>
       </c>
       <c r="E116" t="s">
         <v>93</v>
@@ -29526,7 +29526,7 @@
         <v>1882</v>
       </c>
       <c r="D117" t="s">
-        <v>2051</v>
+        <v>2038</v>
       </c>
       <c r="E117" t="s">
         <v>93</v>
@@ -29645,7 +29645,7 @@
         <v>1882</v>
       </c>
       <c r="D118" t="s">
-        <v>2052</v>
+        <v>2039</v>
       </c>
       <c r="E118" t="s">
         <v>93</v>
@@ -29719,7 +29719,7 @@
         <v>1882</v>
       </c>
       <c r="D119" t="s">
-        <v>2053</v>
+        <v>2040</v>
       </c>
       <c r="E119" t="s">
         <v>93</v>

</xml_diff>